<commit_message>
using arrival time instead of admission in the text, put all plots in the paper
</commit_message>
<xml_diff>
--- a/table/table.xlsx
+++ b/table/table.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Dropbox/Research/1.Forecasting for social good/Healthcare/8.hourly-emergency-care-Bhaman-Ivan-Jethro/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7E4C60-52F0-1548-8477-F38B515C2B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED59177-8A77-2345-AD70-2E4170C23F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hourly!$A$1:$J$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hourly!$A$1:$J$14</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
   <si>
     <t>McCarthy 
 2008</t>
@@ -204,10 +204,7 @@
     <t>Poisson regression</t>
   </si>
   <si>
-    <t xml:space="preserve"> Multiple                                                                           </t>
-  </si>
-  <si>
-    <t>seasonality</t>
+    <t xml:space="preserve"> Multiple seasonality                                                                           </t>
   </si>
 </sst>
 </file>
@@ -578,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBE0282-3BD6-7246-955A-41445ED65893}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="J4" sqref="J3:J4"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -594,10 +591,11 @@
     <col min="6" max="6" width="49.1640625" style="4" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.33203125" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="4"/>
+    <col min="9" max="9" width="39" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="88" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -626,182 +624,201 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2008</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
-        <v>2008</v>
+        <v>2019</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>49</v>
+        <v>30</v>
+      </c>
+      <c r="E3" s="4">
+        <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="4">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2014</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2009</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1">
+        <v>2007</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E8" s="4">
         <v>3</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2013</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2009</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="4">
-        <v>4</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2007</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>43</v>
@@ -812,83 +829,83 @@
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C9" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E9" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E10" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="E11" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>43</v>
@@ -897,27 +914,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>43</v>
@@ -926,31 +940,14 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2012</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>43</v>
-      </c>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -958,22 +955,13 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
McCarthy discussion and minor correction up to GAMLSS section
</commit_message>
<xml_diff>
--- a/table/table.xlsx
+++ b/table/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Dropbox/Research/1.Forecasting for social good/Healthcare/8.hourly-emergency-care-Bhaman-Ivan-Jethro/table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/jethro_browell_glasgow_ac_uk/Documents/GItHub/hourly-emergency-care/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3AAB984-016A-4443-82F4-F02E502CCD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E3AAB984-016A-4443-82F4-F02E502CCD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E054D2FF-08BD-4F5E-AB90-CBC062B44F1D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34060" windowHeight="18420" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly" sheetId="3" r:id="rId1"/>
@@ -28,12 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
   <si>
     <t>ED arrivals</t>
-  </si>
-  <si>
-    <t>95% CI</t>
   </si>
   <si>
     <t>MAPE</t>
@@ -179,9 +176,6 @@
     <t xml:space="preserve"> Length</t>
   </si>
   <si>
-    <t>2 years</t>
-  </si>
-  <si>
     <t>Metric</t>
   </si>
   <si>
@@ -204,6 +198,12 @@
   </si>
   <si>
     <t xml:space="preserve">McCarthy </t>
+  </si>
+  <si>
+    <t>Calibration</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -577,55 +577,55 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.69921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.19921875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="49.1640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="49.19921875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.296875" style="4" customWidth="1"/>
     <col min="9" max="9" width="39" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="4"/>
+    <col min="10" max="16384" width="10.796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="88" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
         <v>2020</v>
@@ -634,27 +634,27 @@
         <v>0</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" s="4">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1">
         <v>2019</v>
@@ -663,27 +663,27 @@
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="4">
         <v>5</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1">
         <v>2017</v>
@@ -692,56 +692,56 @@
         <v>0</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="4">
         <v>3</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>2014</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1">
         <v>2013</v>
@@ -750,111 +750,111 @@
         <v>0</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="1">
         <v>2012</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>2009</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="4">
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>2009</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="4">
         <v>2</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1">
         <v>2008</v>
@@ -863,56 +863,56 @@
         <v>0</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>48</v>
+        <v>56</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H10" s="4" t="s">
         <v>42</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>2007</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1">
         <v>2006</v>
@@ -921,25 +921,25 @@
         <v>0</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="4">
         <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
@@ -948,14 +948,14 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>

</xml_diff>

<commit_message>
a draft from Bahman to pass to Ivan to go through a final round of reading and improving.
</commit_message>
<xml_diff>
--- a/table/table.xlsx
+++ b/table/table.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/jethro_browell_glasgow_ac_uk/Documents/GItHub/hourly-emergency-care/table/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bahmanrostami-tabar/Documents/Research/hourly-emergency-care/table/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{E3AAB984-016A-4443-82F4-F02E502CCD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E054D2FF-08BD-4F5E-AB90-CBC062B44F1D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3C6503-7647-8E48-9EE1-0AA9A017BF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{A8786D4A-E8AF-FD44-8516-BC1B3AC09EAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hourly" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hourly!$A$1:$J$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hourly!$A$1:$J$15</definedName>
   </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="70">
   <si>
     <t>ED arrivals</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>RMSE</t>
-  </si>
-  <si>
-    <t>1,2,4,8,24 hours</t>
   </si>
   <si>
     <t>RMSE, ME</t>
@@ -135,9 +132,6 @@
     <t xml:space="preserve">VAR;  Holt winters </t>
   </si>
   <si>
-    <t>Regression; ARIMA; Exponential smoothing</t>
-  </si>
-  <si>
     <t>Binary regression</t>
   </si>
   <si>
@@ -194,16 +188,62 @@
     <t>Poisson regression</t>
   </si>
   <si>
-    <t xml:space="preserve"> Multiple seasonality                                                                           </t>
-  </si>
-  <si>
     <t xml:space="preserve">McCarthy </t>
   </si>
   <si>
-    <t>Calibration</t>
-  </si>
-  <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>4 years</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>3 years</t>
+  </si>
+  <si>
+    <t>2 years</t>
+  </si>
+  <si>
+    <t>Cheng et al.</t>
+  </si>
+  <si>
+    <t>ED visits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h to 4 h
+</t>
+  </si>
+  <si>
+    <t>1,2,4,8,24 h</t>
+  </si>
+  <si>
+    <t>1 year</t>
+  </si>
+  <si>
+    <t>MSE, MAE, MAPE, Prediction interval coverage</t>
+  </si>
+  <si>
+    <t>Prediction interval coverage</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SARIMAX, Holt-Winters, VAR, ARIMA</t>
+  </si>
+  <si>
+    <t>Double Exponential Smoothing; Additive Holt Winter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Seasonality                                                                           </t>
+  </si>
+  <si>
+    <t>Multiple</t>
+  </si>
+  <si>
+    <t>Single</t>
   </si>
 </sst>
 </file>
@@ -246,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -254,11 +294,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,397 +617,427 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBE0282-3BD6-7246-955A-41445ED65893}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.19921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.69921875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="4" customWidth="1"/>
-    <col min="6" max="6" width="49.19921875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="18.296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.296875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="39" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="10.796875" style="4"/>
+    <col min="1" max="1" width="16.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="49.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="I1" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5">
         <v>2020</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="4">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2019</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2019</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="5">
+        <v>2017</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2014</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2013</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="4">
+      <c r="G7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>2009</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="5">
+        <v>2009</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5">
+        <v>2008</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1">
-        <v>2017</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="68" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2007</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5">
+        <v>2006</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="4">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1">
-        <v>2014</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="1">
-        <v>2013</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2012</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1">
-        <v>2009</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="4">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2009</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="4">
-        <v>2</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2008</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="4">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2007</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E11" s="1">
-        <v>2</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2006</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I13" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I15">
-    <sortCondition descending="1" ref="B1:B15"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:I16">
+    <sortCondition descending="1" ref="B1:B16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>